<commit_message>
use a monthly attendance rate assumption
</commit_message>
<xml_diff>
--- a/inst/exdata/sampleDataPHIC.xlsx
+++ b/inst/exdata/sampleDataPHIC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requirement" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="115">
   <si>
     <t xml:space="preserve">activity</t>
   </si>
@@ -119,9 +119,6 @@
     <t xml:space="preserve">field</t>
   </si>
   <si>
-    <t xml:space="preserve">attendance</t>
-  </si>
-  <si>
     <t xml:space="preserve">status</t>
   </si>
   <si>
@@ -186,6 +183,42 @@
   </si>
   <si>
     <t xml:space="preserve">dcc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a_12</t>
   </si>
   <si>
     <t xml:space="preserve">S-240</t>
@@ -346,7 +379,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="MM/DD/YYYY"/>
+    <numFmt numFmtId="167" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -440,12 +473,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -461,7 +494,7 @@
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.15"/>
@@ -471,7 +504,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="8" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -634,10 +667,9 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,27 +735,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD6"/>
+  <dimension ref="A1:AO6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U19" activeCellId="0" sqref="U19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AG1" activeCellId="0" sqref="AG1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="5" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="13.02"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="30" min="12" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="32" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="5" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="13.02"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="29" min="11" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="31" style="1" width="11.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -740,21 +772,21 @@
         <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>32</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>34</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -799,7 +831,7 @@
       <c r="Y1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="4" t="s">
         <v>49</v>
       </c>
       <c r="AA1" s="4" t="s">
@@ -808,49 +840,82 @@
       <c r="AB1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="0" t="s">
         <v>53</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="G2" s="1" t="n">
         <v>14000</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J2" s="5" t="n">
+      <c r="H2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="5" t="n">
         <v>41197</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="L2" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>61</v>
+        <v>72</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="O2" s="1" t="n">
         <v>1</v>
@@ -885,325 +950,490 @@
       <c r="Y2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="Z2" s="1" t="n">
-        <v>1</v>
+      <c r="AC2" s="1" t="n">
+        <v>14000</v>
       </c>
       <c r="AD2" s="1" t="n">
-        <v>14000</v>
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO2" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>1</v>
+        <v>72</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <v>41502</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J3" s="5" t="n">
-        <v>41502</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="O3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="P3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="R3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="S3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="U3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="V3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="W3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="X3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>11</v>
+      <c r="AD3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO3" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>1</v>
+        <v>72</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>42595</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J4" s="5" t="n">
-        <v>42595</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="P4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="R4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="S4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="U4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="V4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="W4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="X4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD4" s="1" t="s">
-        <v>12</v>
+      <c r="AD4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO4" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>1</v>
+        <v>72</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v>43101</v>
+      </c>
+      <c r="J5" s="5" t="n">
+        <v>43465</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J5" s="5" t="n">
-        <v>43101</v>
-      </c>
-      <c r="K5" s="5" t="n">
-        <v>43465</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="P5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="R5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="S5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="U5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="V5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="W5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="X5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="1" t="s">
-        <v>13</v>
+      <c r="AD5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO5" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>1</v>
+        <v>72</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>43101</v>
+      </c>
+      <c r="J6" s="5" t="n">
+        <v>43465</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J6" s="5" t="n">
-        <v>43101</v>
-      </c>
-      <c r="K6" s="5" t="n">
-        <v>43465</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="O6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="P6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="R6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="S6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="U6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="V6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="W6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="X6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="1" t="s">
-        <v>14</v>
+      <c r="AD6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO6" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1228,27 +1458,26 @@
       <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1259,10 +1488,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,10 +1502,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1287,10 +1516,10 @@
         <v>25</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1301,10 +1530,10 @@
         <v>29</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1315,10 +1544,10 @@
         <v>30</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1329,10 +1558,10 @@
         <v>31</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1343,10 +1572,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1357,10 +1586,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1371,10 +1600,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,10 +1614,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1399,10 +1628,10 @@
         <v>15</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1413,10 +1642,10 @@
         <v>19</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1427,10 +1656,10 @@
         <v>25</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1441,10 +1670,10 @@
         <v>21</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1455,10 +1684,10 @@
         <v>22</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1469,10 +1698,10 @@
         <v>27</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1483,10 +1712,10 @@
         <v>13</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1497,10 +1726,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1511,10 +1740,10 @@
         <v>2</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1525,10 +1754,10 @@
         <v>30</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1539,10 +1768,10 @@
         <v>24</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1553,10 +1782,10 @@
         <v>25</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1567,10 +1796,10 @@
         <v>30</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1581,10 +1810,10 @@
         <v>31</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1605,29 +1834,26 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>50000</v>
@@ -1638,7 +1864,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>100000</v>
@@ -1649,7 +1875,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>400</v>
@@ -1660,7 +1886,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>400</v>
@@ -1671,7 +1897,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>8000</v>

</xml_diff>